<commit_message>
Computed some results for DAGs
</commit_message>
<xml_diff>
--- a/results/exactResults.xlsx
+++ b/results/exactResults.xlsx
@@ -390,7 +390,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D9" sqref="A1:D9"/>
@@ -686,6 +686,70 @@
         <v>87.49470996856689</v>
       </c>
     </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>datasetUniform_dag10.xlsxbeginOrder</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>0.8348260481567809</v>
+      </c>
+      <c r="C19" t="n">
+        <v>0.165173951843219</v>
+      </c>
+      <c r="D19" t="n">
+        <v>3.852659225463867</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>datasetUniform_dag10.xlsxendOrder</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>0.09736735146161822</v>
+      </c>
+      <c r="C20" t="n">
+        <v>0.9026326485383818</v>
+      </c>
+      <c r="D20" t="n">
+        <v>3.835338115692139</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>datasetUniform_dag20.xlsxbeginOrder</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>0.8239025968423785</v>
+      </c>
+      <c r="C21" t="n">
+        <v>0.1760974031576215</v>
+      </c>
+      <c r="D21" t="n">
+        <v>5.280167579650879</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>datasetUniform_dag20.xlsxendOrder</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>0.4431607686553564</v>
+      </c>
+      <c r="C22" t="n">
+        <v>0.5568392313446436</v>
+      </c>
+      <c r="D22" t="n">
+        <v>8.93315577507019</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>